<commit_message>
账户导入导出逻辑修改。数据库更新sql: ALTER TABLE `t_sys_balance_detail` ADD COLUMN `user_id` VARCHAR ( 32 ) NOT NULL COMMENT '所属用户id' AFTER `balance_main_id`; UPDATE t_sys_balance_detail t SET t.user_id = 'monezhao'; ALTER TABLE `t_sys_balance_detail` CHANGE COLUMN `account_type` `balance_type` varchar(4) NOT NULL COMMENT '账户类型' AFTER `account`;
</commit_message>
<xml_diff>
--- a/balance-java/db/数据库设计(balance_账户明细).xlsx
+++ b/balance-java/db/数据库设计(balance_账户明细).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Github\account-manager\balance-java\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monezhao/Pictures/GitHub/account-manager/balance-java/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211EB070-1964-400E-9F0F-6D355001DDC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E112640-4133-1648-B52E-D4B88FDA8ADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="修订记录" sheetId="17" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
   <si>
     <t>修改日期</t>
   </si>
@@ -126,9 +126,6 @@
     <t>账户类型</t>
   </si>
   <si>
-    <t>account_type</t>
-  </si>
-  <si>
     <t>balanceType</t>
   </si>
   <si>
@@ -195,6 +192,18 @@
   </si>
   <si>
     <t>0 不删除 1 删除</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属用户id</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>balance_type</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -202,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +223,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -221,11 +231,13 @@
       <sz val="10"/>
       <color indexed="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -283,7 +295,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -305,6 +317,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -618,17 +633,17 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="74.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="74.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="4" customWidth="1"/>
     <col min="5" max="6" width="8.5" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -656,31 +671,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.375" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="8.5" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="16.375" style="1"/>
+    <col min="14" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -721,7 +736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="30">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -751,7 +766,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="15">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -784,7 +799,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="30">
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -792,7 +807,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -810,19 +825,19 @@
         <v>30</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="15">
       <c r="B5" s="3">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
@@ -841,261 +856,287 @@
       </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="15">
       <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1">
-        <v>255</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="15">
       <c r="B7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="1">
+        <v>255</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="15">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1">
         <v>32</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B8" s="3">
+      <c r="H8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="15">
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="15">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B9" s="3">
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" ht="15">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>32</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="15">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="15">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" ht="15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B10" s="3">
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1">
-        <v>32</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B11" s="3">
+      <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B12" s="3">
+      <c r="F15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7">
+      <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="24" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:E1048576 E2:E13" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16:E1048576 E2:E14" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"字符型,浮点型,日期型,时间型,整数型,大文本,大文件"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H15:H1048576 H2:H13" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16:H1048576 H2:H14" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"UUID主键,数据库生成主键,前台输入主键,不空,可空"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15:J1048576 I2:J13" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I16:J1048576 I2:J14" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>